<commit_message>
Improve strucutre of some files
</commit_message>
<xml_diff>
--- a/t1_confection/Miscellaneous/A-O_Parametrization.xlsx
+++ b/t1_confection/Miscellaneous/A-O_Parametrization.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\Backups\ndc_cr_30\t1_confection\Miscellaneous\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\relac_tx\t1_confection\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AFE7E4-E617-4B1A-A2EF-245A79EBF151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1C9279-128E-4BF9-8D7B-014904268D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11235" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed Horizon Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Primary Techs" sheetId="2" r:id="rId2"/>
     <sheet name="Secondary Techs" sheetId="3" r:id="rId3"/>
-    <sheet name="Timeslices" sheetId="9" r:id="rId4"/>
+    <sheet name="Capacities" sheetId="9" r:id="rId4"/>
     <sheet name="Yearsplit" sheetId="10" r:id="rId5"/>
     <sheet name="Other_Techs" sheetId="8" r:id="rId6"/>
     <sheet name="Demand Techs" sheetId="4" r:id="rId7"/>
@@ -23400,8 +23400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E931CB-6428-4E6C-8349-D2AB5AC7B8E6}">
   <dimension ref="A1:AR1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23549,7 +23549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA94D47C-FF8F-4E88-9229-D73682906176}">
   <dimension ref="A1:AO1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -38393,6 +38393,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48eed89a-7418-4977-ae3a-838f0fac8ec5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="416d42ac-85ec-40c4-8054-6c816fd4b6a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C341064803B07E4F8A0204BD36BE6D07" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="75815dbc30d6e2c2c6f7db4084dd8576">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48eed89a-7418-4977-ae3a-838f0fac8ec5" xmlns:ns3="416d42ac-85ec-40c4-8054-6c816fd4b6a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62d034e6bb04b5aaada07dd500b11312" ns2:_="" ns3:_="">
     <xsd:import namespace="48eed89a-7418-4977-ae3a-838f0fac8ec5"/>
@@ -38593,27 +38613,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="48eed89a-7418-4977-ae3a-838f0fac8ec5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="416d42ac-85ec-40c4-8054-6c816fd4b6a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30283688-E650-41A1-B570-C5C9EACA287E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6032D1F5-36DA-40E1-9274-38A2F86F910C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="48eed89a-7418-4977-ae3a-838f0fac8ec5"/>
+    <ds:schemaRef ds:uri="416d42ac-85ec-40c4-8054-6c816fd4b6a7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B404AB8C-19FD-4E66-8D91-7A592958A832}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -38630,23 +38649,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6032D1F5-36DA-40E1-9274-38A2F86F910C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="48eed89a-7418-4977-ae3a-838f0fac8ec5"/>
-    <ds:schemaRef ds:uri="416d42ac-85ec-40c4-8054-6c816fd4b6a7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30283688-E650-41A1-B570-C5C9EACA287E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update preprossing to include VariableCost in a new sheet
</commit_message>
<xml_diff>
--- a/t1_confection/Miscellaneous/A-O_Parametrization.xlsx
+++ b/t1_confection/Miscellaneous/A-O_Parametrization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\relac_tx\t1_confection\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1C9279-128E-4BF9-8D7B-014904268D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324ED187-3E4B-479C-844E-827E104FDA48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fixed Horizon Parameters" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,21 @@
     <sheet name="Secondary Techs" sheetId="3" r:id="rId3"/>
     <sheet name="Capacities" sheetId="9" r:id="rId4"/>
     <sheet name="Yearsplit" sheetId="10" r:id="rId5"/>
-    <sheet name="Other_Techs" sheetId="8" r:id="rId6"/>
-    <sheet name="Demand Techs" sheetId="4" r:id="rId7"/>
-    <sheet name="Vehicle Techs" sheetId="6" r:id="rId8"/>
-    <sheet name="Vehicle Groups" sheetId="7" r:id="rId9"/>
-    <sheet name="Transport Fuel Distribution" sheetId="5" r:id="rId10"/>
+    <sheet name="VariableCost" sheetId="11" r:id="rId6"/>
+    <sheet name="Other_Techs" sheetId="8" r:id="rId7"/>
+    <sheet name="Demand Techs" sheetId="4" r:id="rId8"/>
+    <sheet name="Vehicle Techs" sheetId="6" r:id="rId9"/>
+    <sheet name="Vehicle Groups" sheetId="7" r:id="rId10"/>
+    <sheet name="Transport Fuel Distribution" sheetId="5" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Demand Techs'!$A$1:$AO$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Demand Techs'!$A$1:$AO$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Fixed Horizon Parameters'!$A$1:$H$277</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Primary Techs'!$A$1:$AO$231</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Secondary Techs'!$A$1:$AO$161</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Transport Fuel Distribution'!$A$1:$AO$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Vehicle Groups'!$A$1:$AO$21</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Vehicle Techs'!$A$1:$AT$216</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Transport Fuel Distribution'!$A$1:$AO$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Vehicle Groups'!$A$1:$AO$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Vehicle Techs'!$A$1:$AT$216</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="15">
   <si>
     <t>Tech.Type</t>
   </si>
@@ -117,6 +118,9 @@
   </si>
   <si>
     <t>Timeslices</t>
+  </si>
+  <si>
+    <t>Mode.Operation</t>
   </si>
 </sst>
 </file>
@@ -3589,6 +3593,708 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:AO21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:AO21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="41" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="11">
+        <v>2018</v>
+      </c>
+      <c r="J1" s="11">
+        <v>2019</v>
+      </c>
+      <c r="K1" s="11">
+        <v>2020</v>
+      </c>
+      <c r="L1" s="11">
+        <v>2021</v>
+      </c>
+      <c r="M1" s="11">
+        <v>2022</v>
+      </c>
+      <c r="N1" s="11">
+        <v>2023</v>
+      </c>
+      <c r="O1" s="11">
+        <v>2024</v>
+      </c>
+      <c r="P1" s="11">
+        <v>2025</v>
+      </c>
+      <c r="Q1" s="11">
+        <v>2026</v>
+      </c>
+      <c r="R1" s="11">
+        <v>2027</v>
+      </c>
+      <c r="S1" s="11">
+        <v>2028</v>
+      </c>
+      <c r="T1" s="11">
+        <v>2029</v>
+      </c>
+      <c r="U1" s="11">
+        <v>2030</v>
+      </c>
+      <c r="V1" s="11">
+        <v>2031</v>
+      </c>
+      <c r="W1" s="11">
+        <v>2032</v>
+      </c>
+      <c r="X1" s="11">
+        <v>2033</v>
+      </c>
+      <c r="Y1" s="11">
+        <v>2034</v>
+      </c>
+      <c r="Z1" s="11">
+        <v>2035</v>
+      </c>
+      <c r="AA1" s="11">
+        <v>2036</v>
+      </c>
+      <c r="AB1" s="11">
+        <v>2037</v>
+      </c>
+      <c r="AC1" s="11">
+        <v>2038</v>
+      </c>
+      <c r="AD1" s="11">
+        <v>2039</v>
+      </c>
+      <c r="AE1" s="11">
+        <v>2040</v>
+      </c>
+      <c r="AF1" s="11">
+        <v>2041</v>
+      </c>
+      <c r="AG1" s="11">
+        <v>2042</v>
+      </c>
+      <c r="AH1" s="11">
+        <v>2043</v>
+      </c>
+      <c r="AI1" s="11">
+        <v>2044</v>
+      </c>
+      <c r="AJ1" s="11">
+        <v>2045</v>
+      </c>
+      <c r="AK1" s="11">
+        <v>2046</v>
+      </c>
+      <c r="AL1" s="11">
+        <v>2047</v>
+      </c>
+      <c r="AM1" s="11">
+        <v>2048</v>
+      </c>
+      <c r="AN1" s="11">
+        <v>2049</v>
+      </c>
+      <c r="AO1" s="11">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14"/>
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14"/>
+      <c r="AG4" s="14"/>
+      <c r="AH4" s="14"/>
+      <c r="AI4" s="14"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
+      <c r="AO4" s="14"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="14"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="14"/>
+      <c r="AG6" s="14"/>
+      <c r="AH6" s="14"/>
+      <c r="AI6" s="14"/>
+      <c r="AJ6" s="14"/>
+      <c r="AK6" s="14"/>
+      <c r="AL6" s="14"/>
+      <c r="AM6" s="14"/>
+      <c r="AN6" s="14"/>
+      <c r="AO6" s="14"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="14"/>
+      <c r="W8" s="14"/>
+      <c r="X8" s="14"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="14"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="14"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="14"/>
+      <c r="AG8" s="14"/>
+      <c r="AH8" s="14"/>
+      <c r="AI8" s="14"/>
+      <c r="AJ8" s="14"/>
+      <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
+      <c r="AM8" s="14"/>
+      <c r="AN8" s="14"/>
+      <c r="AO8" s="14"/>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="14"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="14"/>
+      <c r="AG10" s="14"/>
+      <c r="AH10" s="14"/>
+      <c r="AI10" s="14"/>
+      <c r="AJ10" s="14"/>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="14"/>
+      <c r="AM10" s="14"/>
+      <c r="AN10" s="14"/>
+      <c r="AO10" s="14"/>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="14"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
+      <c r="AG12" s="14"/>
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="14"/>
+      <c r="AJ12" s="14"/>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="14"/>
+      <c r="AN12" s="14"/>
+      <c r="AO12" s="14"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14"/>
+      <c r="Z14" s="14"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="14"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14"/>
+      <c r="AG14" s="14"/>
+      <c r="AH14" s="14"/>
+      <c r="AI14" s="14"/>
+      <c r="AJ14" s="14"/>
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="14"/>
+      <c r="AN14" s="14"/>
+      <c r="AO14" s="14"/>
+    </row>
+    <row r="15" spans="1:41" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="14"/>
+      <c r="Z16" s="14"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="14"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="14"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="14"/>
+      <c r="AG16" s="14"/>
+      <c r="AH16" s="14"/>
+      <c r="AI16" s="14"/>
+      <c r="AJ16" s="14"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="14"/>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17" s="39"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+      <c r="Y18" s="14"/>
+      <c r="Z18" s="14"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="14"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="14"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="14"/>
+      <c r="AG18" s="14"/>
+      <c r="AH18" s="14"/>
+      <c r="AI18" s="14"/>
+      <c r="AJ18" s="14"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
+      <c r="AM18" s="14"/>
+      <c r="AN18" s="14"/>
+      <c r="AO18" s="14"/>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A20" s="39"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="14"/>
+      <c r="Z20" s="14"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="14"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="14"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="14"/>
+      <c r="AG20" s="14"/>
+      <c r="AH20" s="14"/>
+      <c r="AI20" s="14"/>
+      <c r="AJ20" s="14"/>
+      <c r="AK20" s="14"/>
+      <c r="AL20" s="14"/>
+      <c r="AM20" s="14"/>
+      <c r="AN20" s="14"/>
+      <c r="AO20" s="14"/>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A21" s="39"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AO52"/>
   <sheetViews>
@@ -23400,7 +24106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E931CB-6428-4E6C-8349-D2AB5AC7B8E6}">
   <dimension ref="A1:AR1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -23686,6 +24392,140 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6ED8EC-DC3C-467E-9132-200C14E18297}">
+  <dimension ref="A1:AM1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD85"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1">
+        <v>2021</v>
+      </c>
+      <c r="K1" s="1">
+        <v>2022</v>
+      </c>
+      <c r="L1" s="1">
+        <v>2023</v>
+      </c>
+      <c r="M1" s="1">
+        <v>2024</v>
+      </c>
+      <c r="N1" s="1">
+        <v>2025</v>
+      </c>
+      <c r="O1" s="1">
+        <v>2026</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2027</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>2028</v>
+      </c>
+      <c r="R1" s="1">
+        <v>2029</v>
+      </c>
+      <c r="S1" s="1">
+        <v>2030</v>
+      </c>
+      <c r="T1" s="1">
+        <v>2031</v>
+      </c>
+      <c r="U1" s="1">
+        <v>2032</v>
+      </c>
+      <c r="V1" s="1">
+        <v>2033</v>
+      </c>
+      <c r="W1" s="1">
+        <v>2034</v>
+      </c>
+      <c r="X1" s="1">
+        <v>2035</v>
+      </c>
+      <c r="Y1" s="1">
+        <v>2036</v>
+      </c>
+      <c r="Z1" s="1">
+        <v>2037</v>
+      </c>
+      <c r="AA1" s="1">
+        <v>2038</v>
+      </c>
+      <c r="AB1" s="1">
+        <v>2039</v>
+      </c>
+      <c r="AC1" s="1">
+        <v>2040</v>
+      </c>
+      <c r="AD1" s="1">
+        <v>2041</v>
+      </c>
+      <c r="AE1" s="1">
+        <v>2042</v>
+      </c>
+      <c r="AF1" s="1">
+        <v>2043</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>2044</v>
+      </c>
+      <c r="AH1" s="1">
+        <v>2045</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>2046</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>2047</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>2048</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>2049</v>
+      </c>
+      <c r="AM1" s="1">
+        <v>2050</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43423B30-6FAC-48CF-AB89-BEF88F84D0B8}">
   <dimension ref="A1:AN3"/>
   <sheetViews>
@@ -23916,7 +24756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AO88"/>
   <sheetViews>
@@ -27807,7 +28647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AT216"/>
   <sheetViews>
@@ -37690,718 +38530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AO21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AO21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="41" width="5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="11">
-        <v>2018</v>
-      </c>
-      <c r="J1" s="11">
-        <v>2019</v>
-      </c>
-      <c r="K1" s="11">
-        <v>2020</v>
-      </c>
-      <c r="L1" s="11">
-        <v>2021</v>
-      </c>
-      <c r="M1" s="11">
-        <v>2022</v>
-      </c>
-      <c r="N1" s="11">
-        <v>2023</v>
-      </c>
-      <c r="O1" s="11">
-        <v>2024</v>
-      </c>
-      <c r="P1" s="11">
-        <v>2025</v>
-      </c>
-      <c r="Q1" s="11">
-        <v>2026</v>
-      </c>
-      <c r="R1" s="11">
-        <v>2027</v>
-      </c>
-      <c r="S1" s="11">
-        <v>2028</v>
-      </c>
-      <c r="T1" s="11">
-        <v>2029</v>
-      </c>
-      <c r="U1" s="11">
-        <v>2030</v>
-      </c>
-      <c r="V1" s="11">
-        <v>2031</v>
-      </c>
-      <c r="W1" s="11">
-        <v>2032</v>
-      </c>
-      <c r="X1" s="11">
-        <v>2033</v>
-      </c>
-      <c r="Y1" s="11">
-        <v>2034</v>
-      </c>
-      <c r="Z1" s="11">
-        <v>2035</v>
-      </c>
-      <c r="AA1" s="11">
-        <v>2036</v>
-      </c>
-      <c r="AB1" s="11">
-        <v>2037</v>
-      </c>
-      <c r="AC1" s="11">
-        <v>2038</v>
-      </c>
-      <c r="AD1" s="11">
-        <v>2039</v>
-      </c>
-      <c r="AE1" s="11">
-        <v>2040</v>
-      </c>
-      <c r="AF1" s="11">
-        <v>2041</v>
-      </c>
-      <c r="AG1" s="11">
-        <v>2042</v>
-      </c>
-      <c r="AH1" s="11">
-        <v>2043</v>
-      </c>
-      <c r="AI1" s="11">
-        <v>2044</v>
-      </c>
-      <c r="AJ1" s="11">
-        <v>2045</v>
-      </c>
-      <c r="AK1" s="11">
-        <v>2046</v>
-      </c>
-      <c r="AL1" s="11">
-        <v>2047</v>
-      </c>
-      <c r="AM1" s="11">
-        <v>2048</v>
-      </c>
-      <c r="AN1" s="11">
-        <v>2049</v>
-      </c>
-      <c r="AO1" s="11">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
-      <c r="AF2" s="14"/>
-      <c r="AG2" s="14"/>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="14"/>
-      <c r="AJ2" s="14"/>
-      <c r="AK2" s="14"/>
-      <c r="AL2" s="14"/>
-      <c r="AM2" s="14"/>
-      <c r="AN2" s="14"/>
-      <c r="AO2" s="14"/>
-    </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
-      <c r="AM3" s="14"/>
-      <c r="AN3" s="14"/>
-      <c r="AO3" s="14"/>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
-      <c r="AG4" s="14"/>
-      <c r="AH4" s="14"/>
-      <c r="AI4" s="14"/>
-      <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
-      <c r="AN4" s="14"/>
-      <c r="AO4" s="14"/>
-    </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-    </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
-      <c r="AG6" s="14"/>
-      <c r="AH6" s="14"/>
-      <c r="AI6" s="14"/>
-      <c r="AJ6" s="14"/>
-      <c r="AK6" s="14"/>
-      <c r="AL6" s="14"/>
-      <c r="AM6" s="14"/>
-      <c r="AN6" s="14"/>
-      <c r="AO6" s="14"/>
-    </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-    </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
-      <c r="AG8" s="14"/>
-      <c r="AH8" s="14"/>
-      <c r="AI8" s="14"/>
-      <c r="AJ8" s="14"/>
-      <c r="AK8" s="14"/>
-      <c r="AL8" s="14"/>
-      <c r="AM8" s="14"/>
-      <c r="AN8" s="14"/>
-      <c r="AO8" s="14"/>
-    </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
-      <c r="AG10" s="14"/>
-      <c r="AH10" s="14"/>
-      <c r="AI10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AK10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AM10" s="14"/>
-      <c r="AN10" s="14"/>
-      <c r="AO10" s="14"/>
-    </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
-      <c r="AG12" s="14"/>
-      <c r="AH12" s="14"/>
-      <c r="AI12" s="14"/>
-      <c r="AJ12" s="14"/>
-      <c r="AK12" s="14"/>
-      <c r="AL12" s="14"/>
-      <c r="AM12" s="14"/>
-      <c r="AN12" s="14"/>
-      <c r="AO12" s="14"/>
-    </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-    </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="14"/>
-      <c r="AF14" s="14"/>
-      <c r="AG14" s="14"/>
-      <c r="AH14" s="14"/>
-      <c r="AI14" s="14"/>
-      <c r="AJ14" s="14"/>
-      <c r="AK14" s="14"/>
-      <c r="AL14" s="14"/>
-      <c r="AM14" s="14"/>
-      <c r="AN14" s="14"/>
-      <c r="AO14" s="14"/>
-    </row>
-    <row r="15" spans="1:41" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="14"/>
-      <c r="AG16" s="14"/>
-      <c r="AH16" s="14"/>
-      <c r="AI16" s="14"/>
-      <c r="AJ16" s="14"/>
-      <c r="AK16" s="14"/>
-      <c r="AL16" s="14"/>
-      <c r="AM16" s="14"/>
-      <c r="AN16" s="14"/>
-      <c r="AO16" s="14"/>
-    </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-    </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
-      <c r="AG18" s="14"/>
-      <c r="AH18" s="14"/>
-      <c r="AI18" s="14"/>
-      <c r="AJ18" s="14"/>
-      <c r="AK18" s="14"/>
-      <c r="AL18" s="14"/>
-      <c r="AM18" s="14"/>
-      <c r="AN18" s="14"/>
-      <c r="AO18" s="14"/>
-    </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-      <c r="AB20" s="14"/>
-      <c r="AC20" s="14"/>
-      <c r="AD20" s="14"/>
-      <c r="AE20" s="14"/>
-      <c r="AF20" s="14"/>
-      <c r="AG20" s="14"/>
-      <c r="AH20" s="14"/>
-      <c r="AI20" s="14"/>
-      <c r="AJ20" s="14"/>
-      <c r="AK20" s="14"/>
-      <c r="AL20" s="14"/>
-      <c r="AM20" s="14"/>
-      <c r="AN20" s="14"/>
-      <c r="AO20" s="14"/>
-    </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="48eed89a-7418-4977-ae3a-838f0fac8ec5">
@@ -38410,6 +38539,15 @@
     <TaxCatchAll xmlns="416d42ac-85ec-40c4-8054-6c816fd4b6a7" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38614,20 +38752,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30283688-E650-41A1-B570-C5C9EACA287E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6032D1F5-36DA-40E1-9274-38A2F86F910C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="48eed89a-7418-4977-ae3a-838f0fac8ec5"/>
     <ds:schemaRef ds:uri="416d42ac-85ec-40c4-8054-6c816fd4b6a7"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30283688-E650-41A1-B570-C5C9EACA287E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>